<commit_message>
add bom code in ppe
</commit_message>
<xml_diff>
--- a/src/main/resources/PPE.xlsx
+++ b/src/main/resources/PPE.xlsx
@@ -44,7 +44,7 @@
     <t>SAP ID</t>
   </si>
   <si>
-    <t>BOM ID</t>
+    <t>BOM Code</t>
   </si>
   <si>
     <t>Product Name</t>
@@ -1169,8 +1169,8 @@
   <sheetPr/>
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
remove required quantity from sheet & modify column name to ERP ID
</commit_message>
<xml_diff>
--- a/src/main/resources/PPE.xlsx
+++ b/src/main/resources/PPE.xlsx
@@ -41,7 +41,7 @@
     <t>Plan/Order ID</t>
   </si>
   <si>
-    <t>SAP ID</t>
+    <t>ERP ID</t>
   </si>
   <si>
     <t>BOM Code</t>
@@ -71,13 +71,13 @@
     <t>Production Shop</t>
   </si>
   <si>
-    <t>Shop ID</t>
+    <t>Shop Code</t>
   </si>
   <si>
     <t>Line</t>
   </si>
   <si>
-    <t>Line ID</t>
+    <t>Line Code</t>
   </si>
   <si>
     <t>Start Date</t>
@@ -92,7 +92,7 @@
     <t>End Time</t>
   </si>
   <si>
-    <t>Item ID</t>
+    <t>Item Code</t>
   </si>
   <si>
     <t>Item Name</t>
@@ -1170,7 +1170,7 @@
   <dimension ref="A1:Z28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1186,7 +1186,7 @@
     <col min="9" max="9" width="8.28181818181818" customWidth="1"/>
     <col min="10" max="10" width="13.1454545454545" customWidth="1"/>
     <col min="11" max="11" width="15.7181818181818" customWidth="1"/>
-    <col min="12" max="12" width="7.71818181818182" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
     <col min="13" max="13" width="4.71818181818182" customWidth="1"/>
     <col min="14" max="14" width="25.1454545454545" customWidth="1"/>
     <col min="15" max="15" width="10.4272727272727" style="2" customWidth="1"/>

</xml_diff>

<commit_message>
remove required quantity from sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/PPE.xlsx
+++ b/src/main/resources/PPE.xlsx
@@ -10,7 +10,7 @@
     <sheet name="PPE Format" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PPE Format'!$A$2:$Z$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PPE Format'!$A$2:$Y$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Production Plan Details</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>UOM</t>
-  </si>
-  <si>
-    <t>Required Quantity</t>
   </si>
   <si>
     <t>Store</t>
@@ -1167,10 +1164,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z28"/>
+  <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1199,11 +1196,10 @@
     <col min="22" max="22" width="10" customWidth="1"/>
     <col min="23" max="23" width="15" customWidth="1"/>
     <col min="24" max="24" width="8.28181818181818" customWidth="1"/>
-    <col min="25" max="25" width="17.5727272727273" customWidth="1"/>
-    <col min="26" max="26" width="19.4272727272727" customWidth="1"/>
+    <col min="25" max="25" width="19.4272727272727" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1233,9 +1229,8 @@
       <c r="W1" s="12"/>
       <c r="X1" s="12"/>
       <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:26">
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1311,11 +1306,8 @@
       <c r="Y2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26">
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
@@ -1341,9 +1333,8 @@
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
-    </row>
-    <row r="4" spans="1:26">
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
@@ -1369,9 +1360,8 @@
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-    </row>
-    <row r="5" spans="1:26">
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
@@ -1397,9 +1387,8 @@
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-    </row>
-    <row r="6" spans="1:26">
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
@@ -1425,9 +1414,8 @@
       <c r="W6" s="5"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
-      <c r="Z6" s="5"/>
-    </row>
-    <row r="7" spans="1:26">
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
@@ -1453,9 +1441,8 @@
       <c r="W7" s="5"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
-      <c r="Z7" s="5"/>
-    </row>
-    <row r="8" spans="1:26">
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
@@ -1481,9 +1468,8 @@
       <c r="W8" s="5"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
-    </row>
-    <row r="9" spans="1:26">
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
@@ -1509,9 +1495,8 @@
       <c r="W9" s="5"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
-    </row>
-    <row r="10" spans="1:26">
+    </row>
+    <row r="10" spans="1:25">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
@@ -1537,9 +1522,8 @@
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
-    </row>
-    <row r="11" spans="1:26">
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
@@ -1565,9 +1549,8 @@
       <c r="W11" s="5"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
-    </row>
-    <row r="12" spans="1:26">
+    </row>
+    <row r="12" spans="1:25">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
@@ -1593,9 +1576,8 @@
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
-      <c r="Z12" s="5"/>
-    </row>
-    <row r="13" spans="1:26">
+    </row>
+    <row r="13" spans="1:25">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
@@ -1621,9 +1603,8 @@
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
-      <c r="Z13" s="5"/>
-    </row>
-    <row r="14" spans="1:26">
+    </row>
+    <row r="14" spans="1:25">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
@@ -1649,9 +1630,8 @@
       <c r="W14" s="5"/>
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
-      <c r="Z14" s="5"/>
-    </row>
-    <row r="15" spans="1:26">
+    </row>
+    <row r="15" spans="1:25">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
@@ -1677,9 +1657,8 @@
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
-      <c r="Z15" s="5"/>
-    </row>
-    <row r="16" spans="1:26">
+    </row>
+    <row r="16" spans="1:25">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
@@ -1705,9 +1684,8 @@
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
       <c r="Y16" s="5"/>
-      <c r="Z16" s="5"/>
-    </row>
-    <row r="17" spans="1:26">
+    </row>
+    <row r="17" spans="1:25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -1733,9 +1711,8 @@
       <c r="W17" s="5"/>
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
-      <c r="Z17" s="5"/>
-    </row>
-    <row r="18" spans="1:26">
+    </row>
+    <row r="18" spans="1:25">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
@@ -1761,9 +1738,8 @@
       <c r="W18" s="5"/>
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
-      <c r="Z18" s="5"/>
-    </row>
-    <row r="19" spans="1:26">
+    </row>
+    <row r="19" spans="1:25">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
@@ -1789,9 +1765,8 @@
       <c r="W19" s="5"/>
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
-      <c r="Z19" s="5"/>
-    </row>
-    <row r="20" spans="1:26">
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -1817,9 +1792,8 @@
       <c r="W20" s="5"/>
       <c r="X20" s="5"/>
       <c r="Y20" s="5"/>
-      <c r="Z20" s="5"/>
-    </row>
-    <row r="21" spans="1:26">
+    </row>
+    <row r="21" spans="1:25">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
@@ -1845,9 +1819,8 @@
       <c r="W21" s="5"/>
       <c r="X21" s="5"/>
       <c r="Y21" s="5"/>
-      <c r="Z21" s="5"/>
-    </row>
-    <row r="22" spans="1:26">
+    </row>
+    <row r="22" spans="1:25">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
@@ -1873,9 +1846,8 @@
       <c r="W22" s="5"/>
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
-      <c r="Z22" s="5"/>
-    </row>
-    <row r="23" spans="1:26">
+    </row>
+    <row r="23" spans="1:25">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
@@ -1901,9 +1873,8 @@
       <c r="W23" s="5"/>
       <c r="X23" s="5"/>
       <c r="Y23" s="5"/>
-      <c r="Z23" s="5"/>
-    </row>
-    <row r="24" spans="1:26">
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
@@ -1929,9 +1900,8 @@
       <c r="W24" s="5"/>
       <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
-      <c r="Z24" s="5"/>
-    </row>
-    <row r="25" spans="1:26">
+    </row>
+    <row r="25" spans="1:25">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
@@ -1957,9 +1927,8 @@
       <c r="W25" s="5"/>
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
-      <c r="Z25" s="5"/>
-    </row>
-    <row r="26" spans="1:26">
+    </row>
+    <row r="26" spans="1:25">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
@@ -1985,9 +1954,8 @@
       <c r="W26" s="5"/>
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
-      <c r="Z26" s="5"/>
-    </row>
-    <row r="27" spans="1:26">
+    </row>
+    <row r="27" spans="1:25">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
@@ -2013,9 +1981,8 @@
       <c r="W27" s="5"/>
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
-      <c r="Z27" s="5"/>
-    </row>
-    <row r="28" spans="1:26">
+    </row>
+    <row r="28" spans="1:25">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
@@ -2041,12 +2008,11 @@
       <c r="W28" s="5"/>
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
-      <c r="Z28" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:R1"/>
-    <mergeCell ref="S1:Z1"/>
+    <mergeCell ref="S1:Y1"/>
   </mergeCells>
   <conditionalFormatting sqref="S3:S28">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">

</xml_diff>

<commit_message>
remove columns from PPE line
</commit_message>
<xml_diff>
--- a/src/main/resources/PPE.xlsx
+++ b/src/main/resources/PPE.xlsx
@@ -10,7 +10,7 @@
     <sheet name="PPE Format" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PPE Format'!$A$2:$Y$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PPE Format'!$A$2:$W$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Production Plan Details</t>
   </si>
@@ -105,12 +105,6 @@
   </si>
   <si>
     <t>Attribute</t>
-  </si>
-  <si>
-    <t>UOM</t>
-  </si>
-  <si>
-    <t>Store</t>
   </si>
 </sst>
 </file>
@@ -1164,10 +1158,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Y28"/>
+  <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1195,11 +1189,9 @@
     <col min="21" max="21" width="9.85454545454546" customWidth="1"/>
     <col min="22" max="22" width="10" customWidth="1"/>
     <col min="23" max="23" width="15" customWidth="1"/>
-    <col min="24" max="24" width="8.28181818181818" customWidth="1"/>
-    <col min="25" max="25" width="19.4272727272727" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:23">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1227,10 +1219,8 @@
       <c r="U1" s="12"/>
       <c r="V1" s="12"/>
       <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:25">
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:23">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1300,14 +1290,8 @@
       <c r="W2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="X2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
@@ -1331,10 +1315,8 @@
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-    </row>
-    <row r="4" spans="1:25">
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
@@ -1358,10 +1340,8 @@
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-    </row>
-    <row r="5" spans="1:25">
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
@@ -1385,10 +1365,8 @@
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-    </row>
-    <row r="6" spans="1:25">
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
@@ -1412,10 +1390,8 @@
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-    </row>
-    <row r="7" spans="1:25">
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
@@ -1439,10 +1415,8 @@
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
-    </row>
-    <row r="8" spans="1:25">
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
@@ -1466,10 +1440,8 @@
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-    </row>
-    <row r="9" spans="1:25">
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
@@ -1493,10 +1465,8 @@
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-    </row>
-    <row r="10" spans="1:25">
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
@@ -1520,10 +1490,8 @@
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-    </row>
-    <row r="11" spans="1:25">
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
@@ -1547,10 +1515,8 @@
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-    </row>
-    <row r="12" spans="1:25">
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
@@ -1574,10 +1540,8 @@
       <c r="U12" s="5"/>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
-      <c r="Y12" s="5"/>
-    </row>
-    <row r="13" spans="1:25">
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
@@ -1601,10 +1565,8 @@
       <c r="U13" s="5"/>
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
-      <c r="Y13" s="5"/>
-    </row>
-    <row r="14" spans="1:25">
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
@@ -1628,10 +1590,8 @@
       <c r="U14" s="5"/>
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
-      <c r="Y14" s="5"/>
-    </row>
-    <row r="15" spans="1:25">
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
@@ -1655,10 +1615,8 @@
       <c r="U15" s="5"/>
       <c r="V15" s="5"/>
       <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-    </row>
-    <row r="16" spans="1:25">
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
@@ -1682,10 +1640,8 @@
       <c r="U16" s="5"/>
       <c r="V16" s="5"/>
       <c r="W16" s="5"/>
-      <c r="X16" s="5"/>
-      <c r="Y16" s="5"/>
-    </row>
-    <row r="17" spans="1:25">
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -1709,10 +1665,8 @@
       <c r="U17" s="5"/>
       <c r="V17" s="5"/>
       <c r="W17" s="5"/>
-      <c r="X17" s="5"/>
-      <c r="Y17" s="5"/>
-    </row>
-    <row r="18" spans="1:25">
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
@@ -1736,10 +1690,8 @@
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
       <c r="W18" s="5"/>
-      <c r="X18" s="5"/>
-      <c r="Y18" s="5"/>
-    </row>
-    <row r="19" spans="1:25">
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
@@ -1763,10 +1715,8 @@
       <c r="U19" s="5"/>
       <c r="V19" s="5"/>
       <c r="W19" s="5"/>
-      <c r="X19" s="5"/>
-      <c r="Y19" s="5"/>
-    </row>
-    <row r="20" spans="1:25">
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -1790,10 +1740,8 @@
       <c r="U20" s="5"/>
       <c r="V20" s="5"/>
       <c r="W20" s="5"/>
-      <c r="X20" s="5"/>
-      <c r="Y20" s="5"/>
-    </row>
-    <row r="21" spans="1:25">
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
@@ -1817,10 +1765,8 @@
       <c r="U21" s="5"/>
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
-      <c r="X21" s="5"/>
-      <c r="Y21" s="5"/>
-    </row>
-    <row r="22" spans="1:25">
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
@@ -1844,10 +1790,8 @@
       <c r="U22" s="5"/>
       <c r="V22" s="5"/>
       <c r="W22" s="5"/>
-      <c r="X22" s="5"/>
-      <c r="Y22" s="5"/>
-    </row>
-    <row r="23" spans="1:25">
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
@@ -1871,10 +1815,8 @@
       <c r="U23" s="5"/>
       <c r="V23" s="5"/>
       <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
-      <c r="Y23" s="5"/>
-    </row>
-    <row r="24" spans="1:25">
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
@@ -1898,10 +1840,8 @@
       <c r="U24" s="5"/>
       <c r="V24" s="5"/>
       <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
-      <c r="Y24" s="5"/>
-    </row>
-    <row r="25" spans="1:25">
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
@@ -1925,10 +1865,8 @@
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
       <c r="W25" s="5"/>
-      <c r="X25" s="5"/>
-      <c r="Y25" s="5"/>
-    </row>
-    <row r="26" spans="1:25">
+    </row>
+    <row r="26" spans="1:23">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
@@ -1952,10 +1890,8 @@
       <c r="U26" s="5"/>
       <c r="V26" s="5"/>
       <c r="W26" s="5"/>
-      <c r="X26" s="5"/>
-      <c r="Y26" s="5"/>
-    </row>
-    <row r="27" spans="1:25">
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
@@ -1979,10 +1915,8 @@
       <c r="U27" s="5"/>
       <c r="V27" s="5"/>
       <c r="W27" s="5"/>
-      <c r="X27" s="5"/>
-      <c r="Y27" s="5"/>
-    </row>
-    <row r="28" spans="1:25">
+    </row>
+    <row r="28" spans="1:23">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
@@ -2006,13 +1940,11 @@
       <c r="U28" s="5"/>
       <c r="V28" s="5"/>
       <c r="W28" s="5"/>
-      <c r="X28" s="5"/>
-      <c r="Y28" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:R1"/>
-    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="S1:W1"/>
   </mergeCells>
   <conditionalFormatting sqref="S3:S28">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">

</xml_diff>